<commit_message>
submit vote from tags in comments
</commit_message>
<xml_diff>
--- a/ASP.NET/365ThreeSixty_v3/365ThreeSixty_v3/Uploads/staff.xlsx
+++ b/ASP.NET/365ThreeSixty_v3/365ThreeSixty_v3/Uploads/staff.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>tier</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Will</t>
+  </si>
+  <si>
+    <t>Handle</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E11" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -429,7 +432,7 @@
     <col min="2" max="4" width="15.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -442,8 +445,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -456,8 +462,12 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" t="str">
+        <f>"@"&amp;B2</f>
+        <v>@Jay</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -470,8 +480,12 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E11" si="0">"@"&amp;B3</f>
+        <v>@Karen</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -484,8 +498,12 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>@Kev</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -498,8 +516,12 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>@Adam</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -512,8 +534,12 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>@Dave</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -526,8 +552,12 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>@Lee</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -540,8 +570,12 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>@Matt</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -554,8 +588,12 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>@Sakis</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -568,8 +606,12 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>@Josh</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -581,6 +623,10 @@
       </c>
       <c r="D11">
         <v>1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>@Will</v>
       </c>
     </row>
   </sheetData>

</xml_diff>